<commit_message>
update to new research page
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WORK\PROJECTS\varadsrivastava.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53683CA2-6EB6-4B52-825B-C1DE39A1023F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF04ADFB-A8FE-4352-BC40-2D408D001716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4F452221-23A1-4909-86B9-533D2F758014}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{4F452221-23A1-4909-86B9-533D2F758014}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="1" r:id="rId1"/>
     <sheet name="2022" sheetId="2" r:id="rId2"/>
+    <sheet name="2021" sheetId="3" r:id="rId3"/>
+    <sheet name="2020" sheetId="4" r:id="rId4"/>
+    <sheet name="2019" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,43 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
-  <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>test1desc</t>
-  </si>
-  <si>
-    <t>test2desc</t>
-  </si>
-  <si>
-    <t>images/bmai1.jpg</t>
-  </si>
-  <si>
-    <t>assets/isarticle1.png</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>test3desc</t>
-  </si>
-  <si>
-    <t>test4</t>
-  </si>
-  <si>
-    <t>test4desc</t>
-  </si>
-  <si>
-    <t>images/nma_empathy.jpg</t>
-  </si>
-  <si>
-    <t>images/neuromatch.png</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>title</t>
   </si>
@@ -71,6 +38,105 @@
   </si>
   <si>
     <t>image</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>I'll be auditing the CSE486 M20 course on 'Intro to Neural and Cognitive Modeling' of Prof. Bapi Raju at IIIT Hyderabad.</t>
+  </si>
+  <si>
+    <t>“How Spike based Neuromorphic Computing can help monitor Social Distancing Efficiently”. IEEE Brain Sponsored Conference on Computational Neuroscience; Presenting poster of an application of my research on energy efficient object detection. (Was the only other person from India)</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>2020_paper.JPG</t>
+  </si>
+  <si>
+    <t>Article published in Intel A.I. Student Ambassadors Publication!</t>
+  </si>
+  <si>
+    <t>One of my first articles on Intel BrainIAK has been published! Follow this link to read it for free! https://link.medium.com/EQnuldxKp4</t>
+  </si>
+  <si>
+    <t>2020_article.png</t>
+  </si>
+  <si>
+    <t>Worked on Social Cognition aspect of the Human Connectome Project under Dr. Marlene Cohen (CMU and University of Pittsburgh) and Dr. Laura Mikula (York University)</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>2020_nma_empathy.jpg</t>
+  </si>
+  <si>
+    <t>Selected in Facebook Reality Labs Sponsored Neuromatch Academy in the Interactive Track! Yay!</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>2020_neuromatch.png</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>2020_bmai5.jpg</t>
+  </si>
+  <si>
+    <t>Attended the International Conference on Human-Computer Interaction, IIIT Allahabad</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>2020_cpczurich.jpg</t>
+  </si>
+  <si>
+    <t>2019_iiita.jpg</t>
+  </si>
+  <si>
+    <t>Attended Computational Neuroscience Lab Meet, IIT Madras</t>
+  </si>
+  <si>
+    <t>Attended Computational Psychiatry Course 2020 Zurich</t>
+  </si>
+  <si>
+    <t>2020_cnslmeet.jpg</t>
+  </si>
+  <si>
+    <t>Neuromatch Academy : Done and Dusted</t>
+  </si>
+  <si>
+    <t>2020_neuromatchdone.jpg</t>
+  </si>
+  <si>
+    <t>QIP CEP Brain Mapping and A.I. Workshop</t>
+  </si>
+  <si>
+    <t>2020_bmai2.jpg</t>
+  </si>
+  <si>
+    <t>Presenting my views at the Brain Mapping and A.I. Workshop at IIT Delhi</t>
+  </si>
+  <si>
+    <t>Interactions with the Cognitive Computing Group, IIIT A: Performing EEG Experiment</t>
+  </si>
+  <si>
+    <t>2019_ccc.jpg</t>
+  </si>
+  <si>
+    <t>Started working in Barclays as a Quantitative Analyst, on behavioural models</t>
+  </si>
+  <si>
+    <t>Got into the Cognitive Science Programme at IIT Delhi! (Yay! After not been able to go across interviews at IIT K and IIT Gn</t>
+  </si>
+  <si>
+    <t>September</t>
   </si>
 </sst>
 </file>
@@ -422,45 +488,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA51111-2732-4884-A79D-9C22C0114BA4}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -470,45 +514,255 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FFC824B-C161-4871-9A45-A2F3246DEF8B}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD1"/>
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="64.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB2A28F8-0EC1-4531-B3AB-74D3EE15D1E4}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E65F8678-A69E-4653-B67D-416FDDF096E4}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="99.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22E7513-6852-4547-BF1B-494E7339ADC7}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="73.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
research space demo update
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WORK\PROJECTS\varadsrivastava.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF04ADFB-A8FE-4352-BC40-2D408D001716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02AF6F9C-1C0A-473E-9E5B-DB82D5A0ACD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{4F452221-23A1-4909-86B9-533D2F758014}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{4F452221-23A1-4909-86B9-533D2F758014}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t>title</t>
   </si>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t>September</t>
+  </si>
+  <si>
+    <t>Started working on LLMs at Barclays</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>Did Internship at RTG Computational Cognition, Germany</t>
   </si>
 </sst>
 </file>
@@ -488,13 +497,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA51111-2732-4884-A79D-9C22C0114BA4}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -505,6 +517,14 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -551,13 +571,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB2A28F8-0EC1-4531-B3AB-74D3EE15D1E4}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="48.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -568,6 +591,14 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -579,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E65F8678-A69E-4653-B67D-416FDDF096E4}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
blog update and about remove card
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WORK\PROJECTS\varadsrivastava.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E72475-96A4-4872-86BD-0180F1D4D49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E83E74-8D01-4664-AD03-64EC46E08B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{4F452221-23A1-4909-86B9-533D2F758014}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4F452221-23A1-4909-86B9-533D2F758014}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
   <si>
     <t>title</t>
   </si>
@@ -195,6 +195,15 @@
   </si>
   <si>
     <t>Selected in Undergraduate Research Initiative (UGRI) at IIT Jodhpur, and worked on Efficient Pedestrian Detection and Edge Computing</t>
+  </si>
+  <si>
+    <t>2024_ihci.jpg</t>
+  </si>
+  <si>
+    <t>2023_waciis.jpg</t>
+  </si>
+  <si>
+    <t>Completed my Master's thesis at the Learning and Information in Networked Complex Systems (LINCS) Group, IIT Delhi</t>
   </si>
 </sst>
 </file>
@@ -551,11 +560,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89999D4-6282-47E7-8C6A-FDFFE866297F}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -574,6 +586,9 @@
       </c>
       <c r="B2" t="s">
         <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -586,7 +601,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -620,6 +635,9 @@
       <c r="B3" t="s">
         <v>34</v>
       </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -628,10 +646,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FFC824B-C161-4871-9A45-A2F3246DEF8B}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,6 +685,14 @@
       </c>
       <c r="C3" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -892,7 +918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22E7513-6852-4547-BF1B-494E7339ADC7}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added ihfc to blog
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WORK\PROJECTS\varadsrivastava.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E83E74-8D01-4664-AD03-64EC46E08B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A713E53-5F8F-44BD-86C9-F865E31F045A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4F452221-23A1-4909-86B9-533D2F758014}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{4F452221-23A1-4909-86B9-533D2F758014}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="59">
   <si>
     <t>title</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t>Completed my Master's thesis at the Learning and Information in Networked Complex Systems (LINCS) Group, IIT Delhi</t>
+  </si>
+  <si>
+    <t>Selected for the Technology Innovation Hub - Cobotics Fellowship!</t>
+  </si>
+  <si>
+    <t>ihfc.PNG</t>
   </si>
 </sst>
 </file>
@@ -560,7 +566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89999D4-6282-47E7-8C6A-FDFFE866297F}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -646,10 +652,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FFC824B-C161-4871-9A45-A2F3246DEF8B}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,6 +699,17 @@
       </c>
       <c r="B4" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>